<commit_message>
test du DAC réussi!
</commit_message>
<xml_diff>
--- a/test_laboratoire.xlsx
+++ b/test_laboratoire.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="test_controle_potentiomètre" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="test_controle_adc12bits" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="test_controle_adc_10bits" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="test_controle_dac16bits" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="58">
   <si>
     <t xml:space="preserve">valeur décimale</t>
   </si>
@@ -133,6 +134,69 @@
   </si>
   <si>
     <t xml:space="preserve">000_0010011000010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0_1111100111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0_1111101000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0_1111101100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0_1111101010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0_1111100001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0_1111100011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0_1111101101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0_1111100110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0_1111100100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0_1111011100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0_1111101011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0_1111011101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valeur binaire </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tension attendue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tension mesurée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(V)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x4000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x7FFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xBFFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x8000</t>
   </si>
 </sst>
 </file>
@@ -246,7 +310,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -268,6 +332,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -343,7 +411,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -613,11 +681,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="515302"/>
-        <c:axId val="67800580"/>
+        <c:axId val="58304151"/>
+        <c:axId val="24941067"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="515302"/>
+        <c:axId val="58304151"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -690,12 +758,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67800580"/>
+        <c:crossAx val="24941067"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67800580"/>
+        <c:axId val="24941067"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -777,7 +845,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="515302"/>
+        <c:crossAx val="58304151"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -825,9 +893,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>261360</xdr:colOff>
+      <xdr:colOff>260640</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -835,8 +903,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5621040" y="334440"/>
-        <a:ext cx="5955840" cy="4187520"/>
+        <a:off x="5468760" y="334440"/>
+        <a:ext cx="4430880" cy="4186800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -862,9 +930,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1091,13 +1160,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1314,20 +1383,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:F13"/>
+  <dimension ref="B3:F11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.9438775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7448979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.7142857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.1785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.219387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.7091836734694"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1354,9 +1421,15 @@
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="2" t="n">
@@ -1365,9 +1438,15 @@
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="2" t="n">
@@ -1376,9 +1455,15 @@
       <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="n">
@@ -1387,9 +1472,15 @@
       <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="n">
@@ -1398,9 +1489,15 @@
       <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="n">
@@ -1409,9 +1506,15 @@
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="2" t="n">
@@ -1420,9 +1523,15 @@
       <c r="C10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="n">
@@ -1431,31 +1540,121 @@
       <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="2" t="n">
+      <c r="D11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B3:D9"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.4948979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="2" t="n">
+      <c r="D5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="6" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>2.3316</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" s="6" t="n">
+        <v>4.6453</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="6" t="n">
+        <v>-2.5</v>
+      </c>
+      <c r="D8" s="6" t="n">
+        <v>-2.3385</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>-5</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>-4.688</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
implémentation des modes de fonctionnement de l'ADC 12 bits (10 bits à venir)
</commit_message>
<xml_diff>
--- a/test_laboratoire.xlsx
+++ b/test_laboratoire.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="test_controle_potentiomètre" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="58">
   <si>
     <t xml:space="preserve">valeur décimale</t>
   </si>
@@ -411,7 +411,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -681,11 +681,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="58304151"/>
-        <c:axId val="24941067"/>
+        <c:axId val="45425970"/>
+        <c:axId val="34449452"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="58304151"/>
+        <c:axId val="45425970"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -758,12 +758,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24941067"/>
+        <c:crossAx val="34449452"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="24941067"/>
+        <c:axId val="34449452"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -845,7 +845,397 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58304151"/>
+        <c:crossAx val="45425970"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>valeurs_datasheet</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>valeurs_datasheet</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>test_controle_dac16bits!$C$5:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>test_controle_dac16bits!$A$5:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>valeurs_expérimentales</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>valeurs_expérimentales</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>test_controle_dac16bits!$D$5:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3316</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.6453</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.3385</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.688</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>test_controle_dac16bits!$A$5:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="85763206"/>
+        <c:axId val="53624136"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="85763206"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Tension (V)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="53624136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="53624136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>numéro du test</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="85763206"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -886,16 +1276,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>554040</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>246600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>260640</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>132120</xdr:rowOff>
+      <xdr:colOff>450720</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>76320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -903,8 +1293,43 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5468760" y="334440"/>
-        <a:ext cx="4430880" cy="4186800"/>
+        <a:off x="1198800" y="2696400"/>
+        <a:ext cx="8586360" cy="3557160"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>70200</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>55080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>228960</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>43200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="4946760" y="542520"/>
+        <a:ext cx="5626080" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -924,16 +1349,15 @@
   </sheetPr>
   <dimension ref="A3:E15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K33" activeCellId="0" sqref="K33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O31" activeCellId="0" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4387755102041"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1160,13 +1584,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1391,10 +1815,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.219387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1566,22 +1992,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:D9"/>
+  <dimension ref="A3:D9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K25" activeCellId="0" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1122448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.4948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9285714285714"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>49</v>
       </c>
@@ -1602,6 +2030,9 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>53</v>
       </c>
@@ -1613,6 +2044,9 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="B6" s="6" t="s">
         <v>54</v>
       </c>
@@ -1624,6 +2058,9 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="B7" s="6" t="s">
         <v>55</v>
       </c>
@@ -1635,6 +2072,9 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="B8" s="6" t="s">
         <v>56</v>
       </c>
@@ -1646,6 +2086,9 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="B9" s="3" t="s">
         <v>57</v>
       </c>
@@ -1664,5 +2107,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test avec modèle  RC est OK
</commit_message>
<xml_diff>
--- a/test_laboratoire.xlsx
+++ b/test_laboratoire.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="test_controle_potentiomètre" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="test_controle_adc12bits" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="test_controle_adc_10bits" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="test_controle_dac16bits" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="test_adc_dac_modele_rc" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="95">
   <si>
     <t xml:space="preserve">valeur décimale</t>
   </si>
@@ -172,15 +173,78 @@
     <t xml:space="preserve">0_1111011101</t>
   </si>
   <si>
+    <t xml:space="preserve">tension appliquée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tension mesurée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9989 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.0029 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.493 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.5 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.511 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.008 ou 0 ou 0.008 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5045 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.5 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.4965 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7546 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7587 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.045 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.037 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.845 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,851 V</t>
+  </si>
+  <si>
     <t xml:space="preserve">valeur binaire </t>
   </si>
   <si>
     <t xml:space="preserve">tension attendue</t>
   </si>
   <si>
-    <t xml:space="preserve">tension mesurée</t>
-  </si>
-  <si>
     <t xml:space="preserve">(V)</t>
   </si>
   <si>
@@ -197,6 +261,54 @@
   </si>
   <si>
     <t xml:space="preserve">0x8000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consigne DAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">courant mesuré</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tension test1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tension test2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,8958 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.74 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,2626 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.43 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,6317 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.65 V </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.018 V </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.4925 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1,044 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.991 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1,5209 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.233 V</t>
   </si>
 </sst>
 </file>
@@ -411,7 +523,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -681,11 +793,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="45425970"/>
-        <c:axId val="34449452"/>
+        <c:axId val="6131087"/>
+        <c:axId val="58391812"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45425970"/>
+        <c:axId val="6131087"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -758,12 +870,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34449452"/>
+        <c:crossAx val="58391812"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="34449452"/>
+        <c:axId val="58391812"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -845,7 +957,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45425970"/>
+        <c:crossAx val="6131087"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -882,7 +994,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1071,11 +1183,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="85763206"/>
-        <c:axId val="53624136"/>
+        <c:axId val="16751594"/>
+        <c:axId val="1668549"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85763206"/>
+        <c:axId val="16751594"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1148,12 +1260,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53624136"/>
+        <c:crossAx val="1668549"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53624136"/>
+        <c:axId val="1668549"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1235,7 +1347,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85763206"/>
+        <c:crossAx val="16751594"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1283,9 +1395,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>450720</xdr:colOff>
+      <xdr:colOff>450360</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>76320</xdr:rowOff>
+      <xdr:rowOff>75960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1293,8 +1405,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1198800" y="2696400"/>
-        <a:ext cx="8586360" cy="3557160"/>
+        <a:off x="1179720" y="2696400"/>
+        <a:ext cx="8748000" cy="3556800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1318,9 +1430,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>228960</xdr:colOff>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>43200</xdr:rowOff>
+      <xdr:rowOff>42840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1328,8 +1440,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4946760" y="542520"/>
-        <a:ext cx="5626080" cy="3239280"/>
+        <a:off x="4708800" y="542520"/>
+        <a:ext cx="4358880" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1349,15 +1461,16 @@
   </sheetPr>
   <dimension ref="A3:E15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="O31" activeCellId="0" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1579,18 +1692,16 @@
   <dimension ref="B3:G13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.2704081632653"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1807,20 +1918,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:F11"/>
+  <dimension ref="B3:F28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1975,6 +2086,149 @@
       <c r="F11" s="2" t="s">
         <v>45</v>
       </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2000,10 +2254,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2011,22 +2266,22 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2034,7 +2289,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>0</v>
@@ -2048,7 +2303,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="C6" s="6" t="n">
         <v>2.5</v>
@@ -2062,7 +2317,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="C7" s="6" t="n">
         <v>5</v>
@@ -2076,7 +2331,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="C8" s="6" t="n">
         <v>-2.5</v>
@@ -2090,7 +2345,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>-5</v>
@@ -2109,4 +2364,112 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B3:E10"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="n">
+        <v>-0.507</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
tests du générateur d'onde triangulaire, évantuelle modification du module de test
</commit_message>
<xml_diff>
--- a/test_laboratoire.xlsx
+++ b/test_laboratoire.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="95">
   <si>
     <t xml:space="preserve">valeur décimale</t>
   </si>
@@ -272,10 +272,10 @@
     <t xml:space="preserve">tension test1</t>
   </si>
   <si>
-    <t xml:space="preserve">tension test2</t>
-  </si>
-  <si>
     <t xml:space="preserve">1,8958 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?</t>
   </si>
   <si>
     <t xml:space="preserve">-0.74 V</t>
@@ -523,7 +523,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -793,11 +793,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="6131087"/>
-        <c:axId val="58391812"/>
+        <c:axId val="26902369"/>
+        <c:axId val="10146413"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="6131087"/>
+        <c:axId val="26902369"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -870,12 +870,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58391812"/>
+        <c:crossAx val="10146413"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="58391812"/>
+        <c:axId val="10146413"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -957,7 +957,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6131087"/>
+        <c:crossAx val="26902369"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -994,7 +994,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1183,11 +1183,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="16751594"/>
-        <c:axId val="1668549"/>
+        <c:axId val="9285735"/>
+        <c:axId val="62619499"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="16751594"/>
+        <c:axId val="9285735"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1260,12 +1260,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1668549"/>
+        <c:crossAx val="62619499"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1668549"/>
+        <c:axId val="62619499"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1347,7 +1347,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16751594"/>
+        <c:crossAx val="9285735"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1395,9 +1395,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>450360</xdr:colOff>
+      <xdr:colOff>450000</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>75960</xdr:rowOff>
+      <xdr:rowOff>75600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1405,8 +1405,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1179720" y="2696400"/>
-        <a:ext cx="8748000" cy="3556800"/>
+        <a:off x="1170360" y="2696400"/>
+        <a:ext cx="8623440" cy="3556440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1430,9 +1430,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:colOff>228240</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>42840</xdr:rowOff>
+      <xdr:rowOff>42480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1440,8 +1440,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4708800" y="542520"/>
-        <a:ext cx="4358880" cy="3238920"/>
+        <a:off x="4651560" y="542520"/>
+        <a:ext cx="4291920" cy="3238560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1467,10 +1467,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1697,11 +1697,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1926,12 +1928,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.6275510204082"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2254,11 +2254,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2371,19 +2371,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:E10"/>
+  <dimension ref="B3:D10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2396,15 +2395,14 @@
       <c r="D3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>84</v>
       </c>
@@ -2413,7 +2411,9 @@
       <c r="B5" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>86</v>
       </c>
@@ -2422,7 +2422,9 @@
       <c r="B6" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>88</v>
       </c>
@@ -2431,7 +2433,9 @@
       <c r="B7" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>89</v>
       </c>
@@ -2440,7 +2444,9 @@
       <c r="B8" s="2" t="n">
         <v>-0.507</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>90</v>
       </c>
@@ -2449,7 +2455,9 @@
       <c r="B9" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>92</v>
       </c>
@@ -2458,7 +2466,9 @@
       <c r="B10" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="D10" s="2" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
générateur d'onde sin fonctionnel + débute onde tri pulsée
</commit_message>
<xml_diff>
--- a/test_laboratoire.xlsx
+++ b/test_laboratoire.xlsx
@@ -5,14 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="test_controle_potentiomètre" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="test_controle_adc12bits" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="test_controle_adc_10bits" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="test_controle_dac16bits" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="test_adc_dac_modele_rc" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="test_controle_potentiomètre (4 mai 2017)" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="test_controle_adc12bits (11 mai 2017)" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="test_controle_adc_10bits (15 mai 2017)" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="test_controle_dac16bits(17 mai 2017)" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="test_adc_dac_resistance (31 mai 2017)" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="79">
   <si>
     <t xml:space="preserve">valeur décimale</t>
   </si>
@@ -261,54 +261,6 @@
   </si>
   <si>
     <t xml:space="preserve">0x8000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">consigne DAC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">courant mesuré</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tension test1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,8958 V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.74 V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,2626 V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.43 V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,6317 V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.65 V </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.018 V </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.4925 V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1,044 V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.991 V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1,5209 V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.233 V</t>
   </si>
 </sst>
 </file>
@@ -319,7 +271,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -342,6 +294,87 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -359,20 +392,77 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -397,7 +487,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -421,13 +511,61 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -435,45 +573,61 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="22">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFB3B3B3"/>
@@ -485,7 +639,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -501,7 +655,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -577,7 +731,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>test_controle_potentiomètre!$A$5:$A$15</c:f>
+              <c:f>'test_controle_potentiomètre (4 mai 2017)'!$A$5:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -619,7 +773,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>test_controle_potentiomètre!$D$5:$D$15</c:f>
+              <c:f>'test_controle_potentiomètre (4 mai 2017)'!$D$5:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -706,7 +860,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>test_controle_potentiomètre!$A$4:$A$15</c:f>
+              <c:f>'test_controle_potentiomètre (4 mai 2017)'!$A$4:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -751,7 +905,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>test_controle_potentiomètre!$C$5:$C$15</c:f>
+              <c:f>'test_controle_potentiomètre (4 mai 2017)'!$C$5:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -793,11 +947,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="26902369"/>
-        <c:axId val="10146413"/>
+        <c:axId val="71433648"/>
+        <c:axId val="80547664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="26902369"/>
+        <c:axId val="71433648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -870,12 +1024,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10146413"/>
+        <c:crossAx val="80547664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="10146413"/>
+        <c:axId val="80547664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -957,7 +1111,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26902369"/>
+        <c:crossAx val="71433648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1045,7 +1199,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>test_controle_dac16bits!$C$5:$C$9</c:f>
+              <c:f>'test_controle_dac16bits(17 mai 2017)'!$C$5:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1069,7 +1223,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>test_controle_dac16bits!$A$5:$A$9</c:f>
+              <c:f>'test_controle_dac16bits(17 mai 2017)'!$A$5:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1135,7 +1289,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>test_controle_dac16bits!$D$5:$D$9</c:f>
+              <c:f>'test_controle_dac16bits(17 mai 2017)'!$D$5:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1159,7 +1313,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>test_controle_dac16bits!$A$5:$A$9</c:f>
+              <c:f>'test_controle_dac16bits(17 mai 2017)'!$A$5:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1183,11 +1337,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="9285735"/>
-        <c:axId val="62619499"/>
+        <c:axId val="4202418"/>
+        <c:axId val="83653367"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="9285735"/>
+        <c:axId val="4202418"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1260,12 +1414,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62619499"/>
+        <c:crossAx val="83653367"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="62619499"/>
+        <c:axId val="83653367"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1347,7 +1501,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9285735"/>
+        <c:crossAx val="4202418"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1395,9 +1549,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>450000</xdr:colOff>
+      <xdr:colOff>449280</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>75600</xdr:rowOff>
+      <xdr:rowOff>74880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1406,7 +1560,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1170360" y="2696400"/>
-        <a:ext cx="8623440" cy="3556440"/>
+        <a:ext cx="8622000" cy="3555720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1430,9 +1584,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>228240</xdr:colOff>
+      <xdr:colOff>227520</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>42480</xdr:rowOff>
+      <xdr:rowOff>41760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1440,8 +1594,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4651560" y="542520"/>
-        <a:ext cx="4291920" cy="3238560"/>
+        <a:off x="4653360" y="542520"/>
+        <a:ext cx="4291200" cy="3237840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1461,16 +1615,16 @@
   </sheetPr>
   <dimension ref="A3:E15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="O31" activeCellId="0" sqref="O31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="13.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1675,7 +1829,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1691,19 +1845,19 @@
   </sheetPr>
   <dimension ref="B3:G13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1907,7 +2061,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
@@ -1922,16 +2076,18 @@
   </sheetPr>
   <dimension ref="B3:F28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.6275510204082"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2233,7 +2389,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
@@ -2248,17 +2404,17 @@
   </sheetPr>
   <dimension ref="A3:D9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K25" activeCellId="0" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2357,7 +2513,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
@@ -2371,112 +2527,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:D10"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="15.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.34"/>
   </cols>
-  <sheetData>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="2" t="n">
-        <v>-0.507</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
générateur de forme d'onde top level
tests fonctionnel + simulation
</commit_message>
<xml_diff>
--- a/test_laboratoire.xlsx
+++ b/test_laboratoire.xlsx
@@ -5,14 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="test_controle_potentiomètre (4 mai 2017)" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="test_controle_adc12bits (11 mai 2017)" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="test_controle_adc_10bits (15 mai 2017)" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="test_controle_dac16bits(17 mai 2017)" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="test_adc_dac_resistance (31 mai 2017)" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="test_adc_dac_resistance (1-5 juin 2017)" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="97">
   <si>
     <t xml:space="preserve">valeur décimale</t>
   </si>
@@ -261,15 +261,72 @@
   </si>
   <si>
     <t xml:space="preserve">0x8000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">résistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commande DAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">courant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tension </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tension normalisée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">courant normalisé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tension mesurée </t>
+  </si>
+  <si>
+    <t xml:space="preserve">courant mesuré</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gain courant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Résistance déduite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ohms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">binaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">décimal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mA ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">borne résistance (V)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">résistance (A)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
   <fonts count="18">
     <font>
@@ -442,7 +499,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -486,6 +543,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -560,7 +673,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -586,6 +699,114 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -677,7 +898,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -947,11 +1168,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="71433648"/>
-        <c:axId val="80547664"/>
+        <c:axId val="25376385"/>
+        <c:axId val="28455565"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71433648"/>
+        <c:axId val="25376385"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1024,12 +1245,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80547664"/>
+        <c:crossAx val="28455565"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80547664"/>
+        <c:axId val="28455565"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1111,7 +1332,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71433648"/>
+        <c:crossAx val="25376385"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1148,7 +1369,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1337,11 +1558,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="4202418"/>
-        <c:axId val="83653367"/>
+        <c:axId val="19098010"/>
+        <c:axId val="38551309"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="4202418"/>
+        <c:axId val="19098010"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1414,12 +1635,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83653367"/>
+        <c:crossAx val="38551309"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83653367"/>
+        <c:axId val="38551309"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1501,7 +1722,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4202418"/>
+        <c:crossAx val="19098010"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1549,9 +1770,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>449280</xdr:colOff>
+      <xdr:colOff>448560</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:rowOff>74160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1560,7 +1781,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1170360" y="2696400"/>
-        <a:ext cx="8622000" cy="3555720"/>
+        <a:ext cx="8621280" cy="3555000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1584,9 +1805,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>227520</xdr:colOff>
+      <xdr:colOff>226800</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>41760</xdr:rowOff>
+      <xdr:rowOff>41040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1594,8 +1815,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4653360" y="542520"/>
-        <a:ext cx="4291200" cy="3237840"/>
+        <a:off x="4654080" y="542520"/>
+        <a:ext cx="4290480" cy="3237120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1615,8 +1836,8 @@
   </sheetPr>
   <dimension ref="A3:E15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O31" activeCellId="0" sqref="O31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O31" activeCellId="1" sqref="L19:L25 O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1846,7 +2067,7 @@
   <dimension ref="B3:G13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+      <selection pane="topLeft" activeCell="F16" activeCellId="1" sqref="L19:L25 F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2077,7 +2298,7 @@
   <dimension ref="B3:F28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="1" sqref="L19:L25 E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2405,7 +2626,7 @@
   <dimension ref="A3:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K25" activeCellId="0" sqref="K25"/>
+      <selection pane="topLeft" activeCell="K25" activeCellId="1" sqref="L19:L25 K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2527,20 +2748,1012 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A3:O25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19:L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="15.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.34"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>996.5</v>
+      </c>
+      <c r="B5" s="7" t="n">
+        <v>1.87</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>1010011010110</v>
+      </c>
+      <c r="D5" s="7" t="n">
+        <v>10001011101</v>
+      </c>
+      <c r="E5" s="8" t="n">
+        <v>-931</v>
+      </c>
+      <c r="F5" s="15" t="n">
+        <f aca="false">(4.096/2)*(E5/1024)</f>
+        <v>-1.862</v>
+      </c>
+      <c r="G5" s="8" t="n">
+        <v>-2858</v>
+      </c>
+      <c r="H5" s="16" t="n">
+        <f aca="false">2.5*(G5/(4095))</f>
+        <v>-1.74481074481074</v>
+      </c>
+      <c r="I5" s="7" t="n">
+        <v>-1.815</v>
+      </c>
+      <c r="J5" s="17" t="n">
+        <f aca="false">I5/A5</f>
+        <v>-0.00182137481184145</v>
+      </c>
+      <c r="K5" s="18" t="n">
+        <f aca="false">H5/J5</f>
+        <v>957.963585236313</v>
+      </c>
+      <c r="L5" s="18" t="n">
+        <f aca="false">F5/(H5/1000)</f>
+        <v>1067.1644506648</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="n">
+        <v>996.5</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>1011100110010</v>
+      </c>
+      <c r="D6" s="19" t="n">
+        <v>10101111000</v>
+      </c>
+      <c r="E6" s="20" t="n">
+        <v>-648</v>
+      </c>
+      <c r="F6" s="21" t="n">
+        <f aca="false">(4.096/2)*(E6/1024)</f>
+        <v>-1.296</v>
+      </c>
+      <c r="G6" s="20" t="n">
+        <v>-2254</v>
+      </c>
+      <c r="H6" s="22" t="n">
+        <f aca="false">2.5*(G6/(4095))</f>
+        <v>-1.37606837606838</v>
+      </c>
+      <c r="I6" s="19" t="n">
+        <v>-1.347</v>
+      </c>
+      <c r="J6" s="23" t="n">
+        <f aca="false">I6/A6</f>
+        <v>-0.00135173105870547</v>
+      </c>
+      <c r="K6" s="5" t="n">
+        <f aca="false">H6/J6</f>
+        <v>1018.00455586647</v>
+      </c>
+      <c r="L6" s="5" t="n">
+        <f aca="false">F6/(H6/1000)</f>
+        <v>941.813664596273</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="n">
+        <v>996.5</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>1101100111110</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>11010111011</v>
+      </c>
+      <c r="E7" s="20" t="n">
+        <v>-325</v>
+      </c>
+      <c r="F7" s="21" t="n">
+        <f aca="false">(4.096/2)*(E7/1023)</f>
+        <v>-0.650635386119257</v>
+      </c>
+      <c r="G7" s="20" t="n">
+        <v>-1218</v>
+      </c>
+      <c r="H7" s="22" t="n">
+        <f aca="false">2.5*(G7/(4095))</f>
+        <v>-0.743589743589744</v>
+      </c>
+      <c r="I7" s="19" t="n">
+        <v>-0.6928</v>
+      </c>
+      <c r="J7" s="23" t="n">
+        <f aca="false">I7/A7</f>
+        <v>-0.000695233316608129</v>
+      </c>
+      <c r="K7" s="5" t="n">
+        <f aca="false">H7/J7</f>
+        <v>1069.55424290875</v>
+      </c>
+      <c r="L7" s="5" t="n">
+        <f aca="false">F7/(H7/1000)</f>
+        <v>874.992415815553</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="n">
+        <v>996.5</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>1111101000111</v>
+      </c>
+      <c r="D8" s="19" t="n">
+        <v>11111111000</v>
+      </c>
+      <c r="E8" s="20" t="n">
+        <v>-8</v>
+      </c>
+      <c r="F8" s="21" t="n">
+        <f aca="false">(4.096/2)*(E8/1023)</f>
+        <v>-0.0160156402737048</v>
+      </c>
+      <c r="G8" s="20" t="n">
+        <v>-185</v>
+      </c>
+      <c r="H8" s="22" t="n">
+        <f aca="false">2.5*(G8/(4095))</f>
+        <v>-0.112942612942613</v>
+      </c>
+      <c r="I8" s="19" t="n">
+        <v>-0.0461</v>
+      </c>
+      <c r="J8" s="23" t="n">
+        <f aca="false">I8/A8</f>
+        <v>-4.62619167084797E-005</v>
+      </c>
+      <c r="K8" s="5" t="n">
+        <f aca="false">H8/J8</f>
+        <v>2441.37340124325</v>
+      </c>
+      <c r="L8" s="5" t="n">
+        <f aca="false">F8/(H8/1000)</f>
+        <v>141.803344693667</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="n">
+        <v>996.5</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>1011110011</v>
+      </c>
+      <c r="D9" s="19" t="n">
+        <v>11110111</v>
+      </c>
+      <c r="E9" s="20" t="n">
+        <v>247</v>
+      </c>
+      <c r="F9" s="21" t="n">
+        <f aca="false">(4.096/2)*(E9/1023)</f>
+        <v>0.494482893450635</v>
+      </c>
+      <c r="G9" s="20" t="n">
+        <v>755</v>
+      </c>
+      <c r="H9" s="22" t="n">
+        <f aca="false">2.5*(G9/(4095))</f>
+        <v>0.460927960927961</v>
+      </c>
+      <c r="I9" s="19" t="n">
+        <v>0.466</v>
+      </c>
+      <c r="J9" s="23" t="n">
+        <f aca="false">I9/A9</f>
+        <v>0.000467636728549925</v>
+      </c>
+      <c r="K9" s="5" t="n">
+        <f aca="false">H9/J9</f>
+        <v>985.653890696809</v>
+      </c>
+      <c r="L9" s="5" t="n">
+        <f aca="false">F9/(H9/1000)</f>
+        <v>1072.79864830747</v>
+      </c>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="n">
+        <v>996.5</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>10111100100</v>
+      </c>
+      <c r="D10" s="19" t="n">
+        <v>111110001</v>
+      </c>
+      <c r="E10" s="20" t="n">
+        <v>497</v>
+      </c>
+      <c r="F10" s="21" t="n">
+        <f aca="false">(4.096/2)*(E10/1023)</f>
+        <v>0.99497165200391</v>
+      </c>
+      <c r="G10" s="20" t="n">
+        <v>1508</v>
+      </c>
+      <c r="H10" s="22" t="n">
+        <f aca="false">2.5*(G10/(4095))</f>
+        <v>0.920634920634921</v>
+      </c>
+      <c r="I10" s="19" t="n">
+        <v>0.978</v>
+      </c>
+      <c r="J10" s="23" t="n">
+        <f aca="false">I10/A10</f>
+        <v>0.000981435022579027</v>
+      </c>
+      <c r="K10" s="5" t="n">
+        <f aca="false">H10/J10</f>
+        <v>938.049793878015</v>
+      </c>
+      <c r="L10" s="5" t="n">
+        <f aca="false">F10/(H10/1000)</f>
+        <v>1080.74507028011</v>
+      </c>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="n">
+        <v>996.5</v>
+      </c>
+      <c r="B11" s="11" t="n">
+        <v>-1.5</v>
+      </c>
+      <c r="C11" s="10" t="n">
+        <v>100110000001</v>
+      </c>
+      <c r="D11" s="11" t="n">
+        <v>1011101100</v>
+      </c>
+      <c r="E11" s="13" t="n">
+        <v>748</v>
+      </c>
+      <c r="F11" s="24" t="n">
+        <f aca="false">(4.096/2)*(E11/1023)</f>
+        <v>1.4974623655914</v>
+      </c>
+      <c r="G11" s="13" t="n">
+        <v>2433</v>
+      </c>
+      <c r="H11" s="25" t="n">
+        <f aca="false">2.5*(G11/(4095))</f>
+        <v>1.48534798534799</v>
+      </c>
+      <c r="I11" s="11" t="n">
+        <v>1.487</v>
+      </c>
+      <c r="J11" s="26" t="n">
+        <f aca="false">I11/A11</f>
+        <v>0.00149222277972905</v>
+      </c>
+      <c r="K11" s="27" t="n">
+        <f aca="false">H11/J11</f>
+        <v>995.392916879131</v>
+      </c>
+      <c r="L11" s="27" t="n">
+        <f aca="false">F11/(H11/1000)</f>
+        <v>1008.15592060777</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>465.5</v>
+      </c>
+      <c r="B12" s="7" t="n">
+        <v>1.87</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>1010001110101</v>
+      </c>
+      <c r="D12" s="7" t="n">
+        <v>11110111101</v>
+      </c>
+      <c r="E12" s="8" t="n">
+        <v>-67</v>
+      </c>
+      <c r="F12" s="15" t="n">
+        <f aca="false">(4.096/2)*(E12/1023)</f>
+        <v>-0.134130987292278</v>
+      </c>
+      <c r="G12" s="7" t="n">
+        <v>-2955</v>
+      </c>
+      <c r="H12" s="28" t="n">
+        <f aca="false">2.5*(G12/(4095))</f>
+        <v>-1.8040293040293</v>
+      </c>
+      <c r="I12" s="29" t="n">
+        <v>-0.637</v>
+      </c>
+      <c r="J12" s="17" t="n">
+        <f aca="false">I12/A12</f>
+        <v>-0.00136842105263158</v>
+      </c>
+      <c r="K12" s="18" t="n">
+        <f aca="false">H12/J12</f>
+        <v>1318.32910679065</v>
+      </c>
+      <c r="L12" s="18" t="n">
+        <f aca="false">F12/(H12/1000)</f>
+        <v>74.3507807731813</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="n">
+        <v>465.5</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="C13" s="4" t="n">
+        <v>1010001001110</v>
+      </c>
+      <c r="D13" s="19" t="n">
+        <v>10110101010</v>
+      </c>
+      <c r="E13" s="20" t="n">
+        <v>-598</v>
+      </c>
+      <c r="F13" s="21" t="n">
+        <f aca="false">(4.096/2)*(E13/1023)</f>
+        <v>-1.19716911045943</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>-2994</v>
+      </c>
+      <c r="H13" s="30" t="n">
+        <f aca="false">2.5*(G13/(4095))</f>
+        <v>-1.82783882783883</v>
+      </c>
+      <c r="I13" s="31" t="n">
+        <v>-1.124</v>
+      </c>
+      <c r="J13" s="23" t="n">
+        <f aca="false">I13/A13</f>
+        <v>-0.00241460794844253</v>
+      </c>
+      <c r="K13" s="5" t="n">
+        <f aca="false">H13/J13</f>
+        <v>756.991970070262</v>
+      </c>
+      <c r="L13" s="5" t="n">
+        <f aca="false">F13/(H13/1000)</f>
+        <v>654.964262836524</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="n">
+        <v>465.5</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>1010110110000</v>
+      </c>
+      <c r="D14" s="19" t="n">
+        <v>11010111001</v>
+      </c>
+      <c r="E14" s="20" t="n">
+        <v>-327</v>
+      </c>
+      <c r="F14" s="21" t="n">
+        <f aca="false">(4.096/2)*(E14/1023)</f>
+        <v>-0.654639296187683</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>-2640</v>
+      </c>
+      <c r="H14" s="30" t="n">
+        <f aca="false">2.5*(G14/(4095))</f>
+        <v>-1.61172161172161</v>
+      </c>
+      <c r="I14" s="31" t="n">
+        <v>-0.728</v>
+      </c>
+      <c r="J14" s="23" t="n">
+        <f aca="false">I14/A14</f>
+        <v>-0.00156390977443609</v>
+      </c>
+      <c r="K14" s="5" t="n">
+        <f aca="false">H14/J14</f>
+        <v>1030.57199211045</v>
+      </c>
+      <c r="L14" s="5" t="n">
+        <f aca="false">F14/(H14/1000)</f>
+        <v>406.173926952813</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="n">
+        <v>465.5</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4" t="n">
+        <v>1111011011001</v>
+      </c>
+      <c r="D15" s="19" t="n">
+        <v>11111110100</v>
+      </c>
+      <c r="E15" s="20" t="n">
+        <v>-12</v>
+      </c>
+      <c r="F15" s="21" t="n">
+        <f aca="false">(4.096/2)*(E15/1023)</f>
+        <v>-0.0240234604105572</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>-295</v>
+      </c>
+      <c r="H15" s="30" t="n">
+        <f aca="false">2.5*(G15/(4095))</f>
+        <v>-0.18009768009768</v>
+      </c>
+      <c r="I15" s="31" t="n">
+        <v>-0.0677</v>
+      </c>
+      <c r="J15" s="23" t="n">
+        <f aca="false">I15/A15</f>
+        <v>-0.000145435016111708</v>
+      </c>
+      <c r="K15" s="5" t="n">
+        <f aca="false">H15/J15</f>
+        <v>1238.33781514727</v>
+      </c>
+      <c r="L15" s="5" t="n">
+        <f aca="false">F15/(H15/1000)</f>
+        <v>133.391281872857</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="n">
+        <v>465.5</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="C16" s="4" t="n">
+        <v>11000101010</v>
+      </c>
+      <c r="D16" s="19" t="n">
+        <v>11110010</v>
+      </c>
+      <c r="E16" s="20" t="n">
+        <v>242</v>
+      </c>
+      <c r="F16" s="21" t="n">
+        <f aca="false">(4.096/2)*(E16/1023)</f>
+        <v>0.48447311827957</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>1578</v>
+      </c>
+      <c r="H16" s="30" t="n">
+        <f aca="false">2.5*(G16/(4095))</f>
+        <v>0.963369963369963</v>
+      </c>
+      <c r="I16" s="31" t="n">
+        <v>0.4513</v>
+      </c>
+      <c r="J16" s="23" t="n">
+        <f aca="false">I16/A16</f>
+        <v>0.000969495166487648</v>
+      </c>
+      <c r="K16" s="5" t="n">
+        <f aca="false">H16/J16</f>
+        <v>993.682069463146</v>
+      </c>
+      <c r="L16" s="5" t="n">
+        <f aca="false">F16/(H16/1000)</f>
+        <v>502.894149392862</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="n">
+        <v>465.5</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C17" s="4" t="n">
+        <v>100110011011</v>
+      </c>
+      <c r="D17" s="19" t="n">
+        <v>111101001</v>
+      </c>
+      <c r="E17" s="20" t="n">
+        <v>489</v>
+      </c>
+      <c r="F17" s="21" t="n">
+        <f aca="false">(4.096/2)*(E17/1023)</f>
+        <v>0.978956011730205</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>2459</v>
+      </c>
+      <c r="H17" s="30" t="n">
+        <f aca="false">2.5*(G17/(4095))</f>
+        <v>1.501221001221</v>
+      </c>
+      <c r="I17" s="31" t="n">
+        <v>0.9819</v>
+      </c>
+      <c r="J17" s="23" t="n">
+        <f aca="false">I17/A17</f>
+        <v>0.0021093447905478</v>
+      </c>
+      <c r="K17" s="5" t="n">
+        <f aca="false">H17/J17</f>
+        <v>711.700148760949</v>
+      </c>
+      <c r="L17" s="5" t="n">
+        <f aca="false">F17/(H17/1000)</f>
+        <v>652.106525910564</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="10" t="n">
+        <v>465.5</v>
+      </c>
+      <c r="B18" s="11" t="n">
+        <v>-1.5</v>
+      </c>
+      <c r="C18" s="10" t="n">
+        <v>101111010001</v>
+      </c>
+      <c r="D18" s="11" t="n">
+        <v>1011000001</v>
+      </c>
+      <c r="E18" s="13" t="n">
+        <v>705</v>
+      </c>
+      <c r="F18" s="24" t="n">
+        <f aca="false">(4.096/2)*(E18/1023)</f>
+        <v>1.41137829912023</v>
+      </c>
+      <c r="G18" s="11" t="n">
+        <v>3025</v>
+      </c>
+      <c r="H18" s="32" t="n">
+        <f aca="false">2.5*(G18/(4095))</f>
+        <v>1.84676434676435</v>
+      </c>
+      <c r="I18" s="33" t="n">
+        <v>1.281</v>
+      </c>
+      <c r="J18" s="26" t="n">
+        <f aca="false">I18/A18</f>
+        <v>0.00275187969924812</v>
+      </c>
+      <c r="K18" s="27" t="n">
+        <f aca="false">H18/J18</f>
+        <v>671.091962075569</v>
+      </c>
+      <c r="L18" s="27" t="n">
+        <f aca="false">F18/(H18/1000)</f>
+        <v>764.243852548411</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
+        <v>9948</v>
+      </c>
+      <c r="B19" s="7" t="n">
+        <v>1.87</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>1111010111110</v>
+      </c>
+      <c r="D19" s="7" t="n">
+        <v>10000111010</v>
+      </c>
+      <c r="E19" s="8" t="n">
+        <v>-966</v>
+      </c>
+      <c r="F19" s="15" t="n">
+        <f aca="false">(4.096/2)*(E19/1023)</f>
+        <v>-1.93388856304985</v>
+      </c>
+      <c r="G19" s="7" t="n">
+        <v>-322</v>
+      </c>
+      <c r="H19" s="28" t="n">
+        <f aca="false">2.5*(G19/(4095))</f>
+        <v>-0.196581196581197</v>
+      </c>
+      <c r="I19" s="29" t="n">
+        <v>-1.925</v>
+      </c>
+      <c r="J19" s="17" t="n">
+        <f aca="false">I19/A19</f>
+        <v>-0.000193506232408524</v>
+      </c>
+      <c r="K19" s="18" t="n">
+        <f aca="false">H19/J19</f>
+        <v>1015.89077589078</v>
+      </c>
+      <c r="L19" s="18" t="n">
+        <f aca="false">F19/(H19/1000)</f>
+        <v>9837.60703812317</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="n">
+        <v>9948</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="C20" s="4" t="n">
+        <v>1111100111101</v>
+      </c>
+      <c r="D20" s="19" t="n">
+        <v>10101110111</v>
+      </c>
+      <c r="E20" s="20" t="n">
+        <v>-649</v>
+      </c>
+      <c r="F20" s="21" t="n">
+        <f aca="false">(4.096/2)*(E20/1023)</f>
+        <v>-1.2992688172043</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>-195</v>
+      </c>
+      <c r="H20" s="30" t="n">
+        <f aca="false">2.5*(G20/(4095))</f>
+        <v>-0.119047619047619</v>
+      </c>
+      <c r="I20" s="31" t="n">
+        <v>-1.289</v>
+      </c>
+      <c r="J20" s="23" t="n">
+        <f aca="false">I20/A20</f>
+        <v>-0.000129573783675111</v>
+      </c>
+      <c r="K20" s="5" t="n">
+        <f aca="false">H20/J20</f>
+        <v>918.76316081126</v>
+      </c>
+      <c r="L20" s="5" t="n">
+        <f aca="false">F20/(H20/1000)</f>
+        <v>10913.8580645161</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="n">
+        <v>9948</v>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="C21" s="4" t="n">
+        <v>1111110001011</v>
+      </c>
+      <c r="D21" s="19" t="n">
+        <v>11010110101</v>
+      </c>
+      <c r="E21" s="20" t="n">
+        <v>-331</v>
+      </c>
+      <c r="F21" s="21" t="n">
+        <f aca="false">(4.096/2)*(E21/1023)</f>
+        <v>-0.662647116324536</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>-117</v>
+      </c>
+      <c r="H21" s="30" t="n">
+        <f aca="false">2.5*(G21/(4095))</f>
+        <v>-0.0714285714285714</v>
+      </c>
+      <c r="I21" s="31" t="n">
+        <v>-0.654</v>
+      </c>
+      <c r="J21" s="23" t="n">
+        <f aca="false">I21/A21</f>
+        <v>-6.57418576598311E-005</v>
+      </c>
+      <c r="K21" s="5" t="n">
+        <f aca="false">H21/J21</f>
+        <v>1086.50065530799</v>
+      </c>
+      <c r="L21" s="5" t="n">
+        <f aca="false">F21/(H21/1000)</f>
+        <v>9277.0596285435</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="n">
+        <v>9948</v>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="19" t="n">
+        <v>11111110110</v>
+      </c>
+      <c r="E22" s="20" t="n">
+        <v>-10</v>
+      </c>
+      <c r="F22" s="21" t="n">
+        <f aca="false">(4.096/2)*(E22/1023)</f>
+        <v>-0.020019550342131</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="30" t="n">
+        <f aca="false">2.5*(G22/(4095))</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="31" t="n">
+        <v>-0.017</v>
+      </c>
+      <c r="J22" s="23" t="n">
+        <f aca="false">I22/A22</f>
+        <v>-1.70888620828307E-006</v>
+      </c>
+      <c r="K22" s="5" t="n">
+        <f aca="false">H22/J22</f>
+        <v>-0</v>
+      </c>
+      <c r="L22" s="5" t="e">
+        <f aca="false">F22/(H22/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="n">
+        <v>9948</v>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="C23" s="4" t="n">
+        <v>1011100</v>
+      </c>
+      <c r="D23" s="19" t="n">
+        <v>11110101</v>
+      </c>
+      <c r="E23" s="20" t="n">
+        <v>245</v>
+      </c>
+      <c r="F23" s="21" t="n">
+        <f aca="false">(4.096/2)*(E23/1023)</f>
+        <v>0.490478983382209</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>92</v>
+      </c>
+      <c r="H23" s="30" t="n">
+        <f aca="false">2.5*(G23/(4095))</f>
+        <v>0.0561660561660562</v>
+      </c>
+      <c r="I23" s="31" t="n">
+        <v>0.492</v>
+      </c>
+      <c r="J23" s="23" t="n">
+        <f aca="false">I23/A23</f>
+        <v>4.94571773220748E-005</v>
+      </c>
+      <c r="K23" s="5" t="n">
+        <f aca="false">H23/J23</f>
+        <v>1135.65025760148</v>
+      </c>
+      <c r="L23" s="5" t="n">
+        <f aca="false">F23/(H23/1000)</f>
+        <v>8732.65842152238</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="n">
+        <v>9948</v>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C24" s="4" t="n">
+        <v>10011010</v>
+      </c>
+      <c r="D24" s="19" t="n">
+        <v>111110001</v>
+      </c>
+      <c r="E24" s="20" t="n">
+        <v>497</v>
+      </c>
+      <c r="F24" s="21" t="n">
+        <f aca="false">(4.096/2)*(E24/1023)</f>
+        <v>0.99497165200391</v>
+      </c>
+      <c r="G24" s="2" t="n">
+        <v>154</v>
+      </c>
+      <c r="H24" s="30" t="n">
+        <f aca="false">2.5*(G24/(4095))</f>
+        <v>0.094017094017094</v>
+      </c>
+      <c r="I24" s="31" t="n">
+        <v>1.0027</v>
+      </c>
+      <c r="J24" s="23" t="n">
+        <f aca="false">I24/A24</f>
+        <v>0.000100794129473261</v>
+      </c>
+      <c r="K24" s="5" t="n">
+        <f aca="false">H24/J24</f>
+        <v>932.763589590158</v>
+      </c>
+      <c r="L24" s="5" t="n">
+        <f aca="false">F24/(H24/1000)</f>
+        <v>10582.880298587</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="10" t="n">
+        <v>9948</v>
+      </c>
+      <c r="B25" s="11" t="n">
+        <v>-1.5</v>
+      </c>
+      <c r="C25" s="10" t="n">
+        <v>11011000</v>
+      </c>
+      <c r="D25" s="11" t="n">
+        <v>1011110010</v>
+      </c>
+      <c r="E25" s="13" t="n">
+        <v>754</v>
+      </c>
+      <c r="F25" s="24" t="n">
+        <f aca="false">(4.096/2)*(E25/1023)</f>
+        <v>1.50947409579668</v>
+      </c>
+      <c r="G25" s="11" t="n">
+        <v>216</v>
+      </c>
+      <c r="H25" s="32" t="n">
+        <f aca="false">2.5*(G25/(4095))</f>
+        <v>0.131868131868132</v>
+      </c>
+      <c r="I25" s="33" t="n">
+        <v>1.512</v>
+      </c>
+      <c r="J25" s="26" t="n">
+        <f aca="false">I25/A25</f>
+        <v>0.000151990349819059</v>
+      </c>
+      <c r="K25" s="27" t="n">
+        <f aca="false">H25/J25</f>
+        <v>867.608581894296</v>
+      </c>
+      <c r="L25" s="27" t="n">
+        <f aca="false">F25/(H25/1000)</f>
+        <v>11446.8452264581</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
test des mode de fonctionnemtn de l'ADC 12 bits (implémentation physique) et début de la programmation des modes de fonctionnement de l'ADC 10 bits
</commit_message>
<xml_diff>
--- a/test_laboratoire.xlsx
+++ b/test_laboratoire.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="test_controle_potentiomètre (4 mai 2017)" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,7 @@
     <sheet name="test_controle_adc_10bits (15 mai 2017)" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="test_controle_dac16bits(17 mai 2017)" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="test_adc_dac_resistance (1-5 juin 2017)" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="mode_fonctionnement_adc12bits (9 juin 2017)" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="97">
   <si>
     <t xml:space="preserve">valeur décimale</t>
   </si>
@@ -898,7 +899,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1168,11 +1169,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="25376385"/>
-        <c:axId val="28455565"/>
+        <c:axId val="59605373"/>
+        <c:axId val="38080823"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="25376385"/>
+        <c:axId val="59605373"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1245,12 +1246,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28455565"/>
+        <c:crossAx val="38080823"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="28455565"/>
+        <c:axId val="38080823"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1332,7 +1333,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25376385"/>
+        <c:crossAx val="59605373"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1369,7 +1370,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1558,11 +1559,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="19098010"/>
-        <c:axId val="38551309"/>
+        <c:axId val="31833000"/>
+        <c:axId val="72814845"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="19098010"/>
+        <c:axId val="31833000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1635,12 +1636,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38551309"/>
+        <c:crossAx val="72814845"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="38551309"/>
+        <c:axId val="72814845"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1722,7 +1723,227 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19098010"/>
+        <c:crossAx val="31833000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'mode_fonctionnement_adc12bits (9 juin 2017)'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>tension normalisée</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'mode_fonctionnement_adc12bits (9 juin 2017)'!$A$3:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'mode_fonctionnement_adc12bits (9 juin 2017)'!$C$3:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-0.172771672771673</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.188644688644689</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.204517704517704</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.219169719169719</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="7606824"/>
+        <c:axId val="38174294"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="7606824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="38174294"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="38174294"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="7606824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1770,9 +1991,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>448560</xdr:colOff>
+      <xdr:colOff>448200</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>74160</xdr:rowOff>
+      <xdr:rowOff>73800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1781,7 +2002,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1170360" y="2696400"/>
-        <a:ext cx="8621280" cy="3555000"/>
+        <a:ext cx="8620920" cy="3554640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1805,9 +2026,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>226800</xdr:colOff>
+      <xdr:colOff>226440</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>41040</xdr:rowOff>
+      <xdr:rowOff>40680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1816,7 +2037,42 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="4654080" y="542520"/>
-        <a:ext cx="4290480" cy="3237120"/>
+        <a:ext cx="4290120" cy="3236760"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>596520</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>74160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>666360</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>62640</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="3702600" y="236520"/>
+        <a:ext cx="5759640" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1837,7 +2093,7 @@
   <dimension ref="A3:E15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O31" activeCellId="1" sqref="L19:L25 O31"/>
+      <selection pane="topLeft" activeCell="O31" activeCellId="0" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2067,7 +2323,7 @@
   <dimension ref="B3:G13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="1" sqref="L19:L25 F16"/>
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2298,7 +2554,7 @@
   <dimension ref="B3:F28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="1" sqref="L19:L25 E28"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2626,7 +2882,7 @@
   <dimension ref="A3:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K25" activeCellId="1" sqref="L19:L25 K25"/>
+      <selection pane="topLeft" activeCell="K25" activeCellId="0" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2750,8 +3006,8 @@
   </sheetPr>
   <dimension ref="A3:O25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19:L25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3762,4 +4018,146 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:C11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.81"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>-283</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <f aca="false">2.5*(B3/(4095))</f>
+        <v>-0.172771672771673</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>-309</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <f aca="false">2.5*(B4/(4095))</f>
+        <v>-0.188644688644689</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>-335</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <f aca="false">2.5*(B5/(4095))</f>
+        <v>-0.204517704517704</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>-359</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <f aca="false">2.5*(B6/(4095))</f>
+        <v>-0.219169719169719</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="n">
+        <f aca="false">2.5*(B7/(4095))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>370</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <f aca="false">2.5*(B8/(4095))</f>
+        <v>0.225885225885226</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>92</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <f aca="false">2.5*(B9/(4095))</f>
+        <v>0.0561660561660562</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>-276</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <f aca="false">2.5*(B10/(4095))</f>
+        <v>-0.168498168498168</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>-426</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <f aca="false">2.5*(B11/(4095))</f>
+        <v>-0.26007326007326</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>